<commit_message>
Incorporated smart pointers to achieve proper deallocation; paid attention toobject lifetimes
</commit_message>
<xml_diff>
--- a/projectSchematic.xlsx
+++ b/projectSchematic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasirulelwala/Desktop/Cpp_Projects/Robust Insurance Technology/02. R&amp;D/Udacity C++ Nanodegree/05. Capstone Project/Udacity Capstone Submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01592C2-756E-A54F-950C-CD8862A55937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E10DC8-BD15-4A4B-8BE1-8FBB8415D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1D8D9048-64B2-2347-87E0-EF601C358543}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="132">
   <si>
     <t>ATTRIBUTES</t>
   </si>
@@ -440,6 +440,39 @@
       <t>composition relationship</t>
     </r>
   </si>
+  <si>
+    <t>PORTFOLIO CASH-FLOWS BY VALUATION YEAR</t>
+  </si>
+  <si>
+    <t>This class is a holding class. It holds the following:</t>
+  </si>
+  <si>
+    <t>VECTOR OF TIME-STEP PROJECTION OBJECTS</t>
+  </si>
+  <si>
+    <t>VECTOR OF POLICY OBJECTS</t>
+  </si>
+  <si>
+    <t>VECTOR OF DECREMENTS PROJECTION OBJECTS</t>
+  </si>
+  <si>
+    <t>VECTOR OF CASH-FLOWS PROJECTION OBJECTS</t>
+  </si>
+  <si>
+    <t>VECTOR OF CASH-FLOWS BY VALUATION YEAR PROJECTION obj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have many "PushBack" functions to push policy, time-step </t>
+  </si>
+  <si>
+    <t>and other objects into their respective vectors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLLECTING ALL CASH-FLOWS FROM ALL POLICIES AND </t>
+  </si>
+  <si>
+    <t>GROUPING</t>
+  </si>
 </sst>
 </file>
 
@@ -449,7 +482,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -510,6 +543,11 @@
       <i/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -966,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1018,8 +1056,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -1047,6 +1083,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2033,6 +2075,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Right Arrow 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA096D8-C048-4A6C-9061-183EA65F0952}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="8585200"/>
+          <a:ext cx="7239000" cy="50800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2299,10 +2401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00616593-0D2E-7748-A675-50A19E638C5C}">
-  <dimension ref="B1:R76"/>
+  <dimension ref="B1:Y76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F18" zoomScale="136" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D27" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="P64" sqref="P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2432,7 @@
       <c r="L3" s="42"/>
     </row>
     <row r="4" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="77" t="s">
         <v>119</v>
       </c>
       <c r="H4" s="26" t="s">
@@ -2375,7 +2477,7 @@
       <c r="L7" s="22"/>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C8" s="78"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="30"/>
       <c r="E8" s="31"/>
       <c r="H8" s="28"/>
@@ -2389,8 +2491,8 @@
         <v>2</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="22"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.2">
@@ -2398,8 +2500,8 @@
         <v>3</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="22"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.2">
@@ -2412,8 +2514,8 @@
         <v>4</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="22"/>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.2">
@@ -2426,16 +2528,16 @@
         <v>5</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="22"/>
-      <c r="N12" s="60" t="s">
+      <c r="N12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="62"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="60"/>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C13" s="29"/>
@@ -2445,62 +2547,62 @@
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="22"/>
-      <c r="N13" s="63" t="s">
+      <c r="N13" s="61" t="s">
         <v>0</v>
       </c>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="64"/>
+      <c r="R13" s="62"/>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="7"/>
       <c r="L14" s="22"/>
-      <c r="N14" s="65" t="s">
+      <c r="N14" s="63" t="s">
         <v>62</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="66"/>
+      <c r="R14" s="64"/>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H15" s="28" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="22"/>
-      <c r="N15" s="67"/>
+      <c r="N15" s="65"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="66"/>
+      <c r="R15" s="64"/>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H16" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="22"/>
-      <c r="N16" s="68" t="s">
+      <c r="N16" s="66" t="s">
         <v>52</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="66"/>
+      <c r="R16" s="64"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
@@ -2514,16 +2616,16 @@
         <v>10</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="22"/>
-      <c r="N17" s="69" t="s">
+      <c r="N17" s="67" t="s">
         <v>43</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="66"/>
+      <c r="R17" s="64"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
@@ -2537,16 +2639,16 @@
         <v>13</v>
       </c>
       <c r="I18" s="19"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="2"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="7"/>
       <c r="L18" s="22"/>
-      <c r="N18" s="69" t="s">
+      <c r="N18" s="67" t="s">
         <v>42</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="66"/>
+      <c r="R18" s="64"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="s">
@@ -2560,16 +2662,16 @@
         <v>14</v>
       </c>
       <c r="I19" s="19"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="2"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="7"/>
       <c r="L19" s="22"/>
-      <c r="N19" s="69" t="s">
+      <c r="N19" s="67" t="s">
         <v>47</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="66"/>
+      <c r="R19" s="64"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="28"/>
@@ -2581,16 +2683,16 @@
         <v>15</v>
       </c>
       <c r="I20" s="19"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="2"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="7"/>
       <c r="L20" s="22"/>
-      <c r="N20" s="69" t="s">
+      <c r="N20" s="67" t="s">
         <v>48</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="66"/>
+      <c r="R20" s="64"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="34" t="s">
@@ -2604,16 +2706,16 @@
         <v>16</v>
       </c>
       <c r="I21" s="21"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="2"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="22"/>
-      <c r="N21" s="69" t="s">
+      <c r="N21" s="67" t="s">
         <v>49</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="66"/>
+      <c r="R21" s="64"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
@@ -2628,13 +2730,13 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="22"/>
-      <c r="N22" s="69" t="s">
+      <c r="N22" s="67" t="s">
         <v>44</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="66"/>
+      <c r="R22" s="64"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
@@ -2649,11 +2751,11 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="22"/>
-      <c r="N23" s="67"/>
+      <c r="N23" s="65"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="66"/>
+      <c r="R23" s="64"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="28"/>
@@ -2668,13 +2770,13 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="22"/>
-      <c r="N24" s="63" t="s">
+      <c r="N24" s="61" t="s">
         <v>17</v>
       </c>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
-      <c r="R24" s="64"/>
+      <c r="R24" s="62"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="34" t="s">
@@ -2689,11 +2791,11 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="22"/>
-      <c r="N25" s="67"/>
+      <c r="N25" s="65"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="66"/>
+      <c r="R25" s="64"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="28" t="s">
@@ -2710,13 +2812,13 @@
       <c r="J26" s="35"/>
       <c r="K26" s="13"/>
       <c r="L26" s="22"/>
-      <c r="N26" s="68" t="s">
+      <c r="N26" s="66" t="s">
         <v>58</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="66"/>
+      <c r="R26" s="64"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="34" t="s">
@@ -2731,13 +2833,13 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="22"/>
-      <c r="N27" s="69" t="s">
+      <c r="N27" s="67" t="s">
         <v>45</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
-      <c r="R27" s="66"/>
+      <c r="R27" s="64"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
@@ -2754,13 +2856,13 @@
       <c r="J28" s="4"/>
       <c r="K28" s="5"/>
       <c r="L28" s="22"/>
-      <c r="N28" s="69" t="s">
+      <c r="N28" s="67" t="s">
         <v>37</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
-      <c r="R28" s="66"/>
+      <c r="R28" s="64"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="28"/>
@@ -2775,13 +2877,13 @@
       <c r="J29" s="2"/>
       <c r="K29" s="7"/>
       <c r="L29" s="22"/>
-      <c r="N29" s="69" t="s">
+      <c r="N29" s="67" t="s">
         <v>38</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="66"/>
+      <c r="R29" s="64"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" s="28" t="s">
@@ -2798,13 +2900,13 @@
       <c r="J30" s="9"/>
       <c r="K30" s="10"/>
       <c r="L30" s="22"/>
-      <c r="N30" s="69" t="s">
+      <c r="N30" s="67" t="s">
         <v>39</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="66"/>
+      <c r="R30" s="64"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
@@ -2819,13 +2921,13 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="22"/>
-      <c r="N31" s="69" t="s">
+      <c r="N31" s="67" t="s">
         <v>40</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
-      <c r="R31" s="66"/>
+      <c r="R31" s="64"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="28"/>
@@ -2838,15 +2940,15 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="22"/>
-      <c r="N32" s="69" t="s">
+      <c r="N32" s="67" t="s">
         <v>41</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="66"/>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R32" s="64"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>17</v>
       </c>
@@ -2861,13 +2963,13 @@
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
       <c r="L33" s="27"/>
-      <c r="N33" s="67"/>
+      <c r="N33" s="65"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="66"/>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R33" s="64"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B34" s="28"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -2878,15 +2980,15 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="22"/>
-      <c r="N34" s="70" t="s">
+      <c r="N34" s="68" t="s">
         <v>117</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
-      <c r="R34" s="66"/>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R34" s="64"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B35" s="28" t="s">
         <v>56</v>
       </c>
@@ -2897,17 +2999,17 @@
       <c r="H35" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="2"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="2"/>
       <c r="L35" s="22"/>
-      <c r="N35" s="72"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="74"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="N35" s="70"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="72"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B36" s="28"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2919,7 +3021,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="22"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B37" s="28" t="s">
         <v>111</v>
       </c>
@@ -2934,15 +3036,15 @@
       <c r="J37" s="13"/>
       <c r="K37" s="2"/>
       <c r="L37" s="22"/>
-      <c r="N37" s="60" t="s">
+      <c r="N37" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="O37" s="61"/>
-      <c r="P37" s="61"/>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="62"/>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="60"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B38" s="33" t="s">
         <v>112</v>
       </c>
@@ -2955,15 +3057,15 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="22"/>
-      <c r="N38" s="63" t="s">
+      <c r="N38" s="61" t="s">
         <v>0</v>
       </c>
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
-      <c r="R38" s="64"/>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R38" s="62"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B39" s="29"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
@@ -2976,15 +3078,15 @@
       <c r="J39" s="13"/>
       <c r="K39" s="2"/>
       <c r="L39" s="22"/>
-      <c r="N39" s="65" t="s">
+      <c r="N39" s="63" t="s">
         <v>59</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="66"/>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R39" s="64"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2995,22 +3097,29 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="22"/>
-      <c r="N40" s="65" t="s">
+      <c r="N40" s="63" t="s">
         <v>60</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
-      <c r="R40" s="66"/>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B41" s="60" t="s">
+      <c r="R40" s="64"/>
+      <c r="U40" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="V40" s="24"/>
+      <c r="W40" s="24"/>
+      <c r="X40" s="24"/>
+      <c r="Y40" s="25"/>
+    </row>
+    <row r="41" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B41" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="62"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="60"/>
       <c r="H41" s="39" t="s">
         <v>105</v>
       </c>
@@ -3018,458 +3127,619 @@
       <c r="J41" s="35"/>
       <c r="K41" s="13"/>
       <c r="L41" s="22"/>
-      <c r="N41" s="67"/>
+      <c r="N41" s="65"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
-      <c r="R41" s="66"/>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B42" s="63" t="s">
+      <c r="R41" s="64"/>
+      <c r="U41" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="27"/>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B42" s="61" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
-      <c r="F42" s="64"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="31"/>
-      <c r="N42" s="68" t="s">
+      <c r="F42" s="62"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="22"/>
+      <c r="N42" s="66" t="s">
         <v>52</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
-      <c r="R42" s="66"/>
-    </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B43" s="65" t="s">
+      <c r="R42" s="64"/>
+      <c r="U42" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="22"/>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B43" s="63" t="s">
         <v>106</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="66"/>
-      <c r="N43" s="69" t="s">
+      <c r="F43" s="64"/>
+      <c r="H43" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="81"/>
+      <c r="L43" s="22"/>
+      <c r="N43" s="67" t="s">
         <v>53</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="66"/>
-    </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B44" s="67"/>
+      <c r="R43" s="64"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="22"/>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B44" s="65"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="66"/>
-      <c r="N44" s="69" t="s">
+      <c r="F44" s="64"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="31"/>
+      <c r="N44" s="67" t="s">
         <v>54</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="66"/>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B45" s="68" t="s">
+      <c r="R44" s="64"/>
+      <c r="U44" s="82" t="s">
+        <v>124</v>
+      </c>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="22"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B45" s="66" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="66"/>
-      <c r="N45" s="70"/>
+      <c r="F45" s="64"/>
+      <c r="N45" s="68"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
-      <c r="R45" s="66"/>
-    </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="s">
+      <c r="R45" s="64"/>
+      <c r="U45" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="22"/>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B46" s="65" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="66"/>
-      <c r="N46" s="67" t="s">
+      <c r="F46" s="64"/>
+      <c r="N46" s="65" t="s">
         <v>68</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="66"/>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B47" s="67"/>
+      <c r="R46" s="64"/>
+      <c r="U46" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="22"/>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B47" s="65"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="66"/>
-      <c r="N47" s="67" t="s">
+      <c r="F47" s="64"/>
+      <c r="N47" s="65" t="s">
         <v>70</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="66"/>
-    </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B48" s="63" t="s">
+      <c r="R47" s="64"/>
+      <c r="U47" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="22"/>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B48" s="61" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
-      <c r="F48" s="64"/>
-      <c r="N48" s="67" t="s">
+      <c r="F48" s="62"/>
+      <c r="N48" s="65" t="s">
         <v>70</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="66"/>
-    </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B49" s="67"/>
+      <c r="R48" s="64"/>
+      <c r="U48" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="22"/>
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B49" s="65"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="66"/>
-      <c r="H49" s="60" t="s">
+      <c r="F49" s="64"/>
+      <c r="H49" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="62"/>
-      <c r="N49" s="67" t="s">
+      <c r="I49" s="59"/>
+      <c r="J49" s="59"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="60"/>
+      <c r="N49" s="65" t="s">
         <v>69</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
-      <c r="R49" s="66"/>
-    </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B50" s="68" t="s">
+      <c r="R49" s="64"/>
+      <c r="U49" s="33"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="22"/>
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B50" s="66" t="s">
         <v>58</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="66"/>
-      <c r="H50" s="63" t="s">
+      <c r="F50" s="64"/>
+      <c r="H50" s="61" t="s">
         <v>0</v>
       </c>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
-      <c r="L50" s="64"/>
-      <c r="N50" s="67"/>
+      <c r="L50" s="62"/>
+      <c r="N50" s="65"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="66"/>
-    </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B51" s="67" t="s">
+      <c r="R50" s="64"/>
+      <c r="U50" s="33"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="22"/>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B51" s="65" t="s">
         <v>108</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="66"/>
-      <c r="H51" s="65" t="s">
+      <c r="F51" s="64"/>
+      <c r="H51" s="63" t="s">
         <v>104</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="L51" s="66"/>
-      <c r="N51" s="63" t="s">
+      <c r="L51" s="64"/>
+      <c r="N51" s="61" t="s">
         <v>17</v>
       </c>
       <c r="O51" s="14"/>
       <c r="P51" s="14"/>
       <c r="Q51" s="14"/>
-      <c r="R51" s="64"/>
-    </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B52" s="67" t="s">
+      <c r="R51" s="62"/>
+      <c r="U51" s="28"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+      <c r="Y51" s="22"/>
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B52" s="65" t="s">
         <v>109</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="66"/>
-      <c r="H52" s="65"/>
+      <c r="F52" s="64"/>
+      <c r="H52" s="63"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="66"/>
-      <c r="N52" s="67"/>
+      <c r="L52" s="64"/>
+      <c r="N52" s="65"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
-      <c r="R52" s="66"/>
-    </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B53" s="67"/>
+      <c r="R52" s="64"/>
+      <c r="U52" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="V52" s="14"/>
+      <c r="W52" s="14"/>
+      <c r="X52" s="14"/>
+      <c r="Y52" s="27"/>
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B53" s="65"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="66"/>
-      <c r="H53" s="68" t="s">
+      <c r="F53" s="64"/>
+      <c r="H53" s="66" t="s">
         <v>57</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="66"/>
-      <c r="N53" s="68" t="s">
+      <c r="L53" s="64"/>
+      <c r="N53" s="66" t="s">
         <v>58</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="66"/>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B54" s="67" t="s">
+      <c r="R53" s="64"/>
+      <c r="U53" s="28"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2"/>
+      <c r="Y53" s="22"/>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B54" s="65" t="s">
         <v>110</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="66"/>
-      <c r="H54" s="67" t="s">
+      <c r="F54" s="64"/>
+      <c r="H54" s="65" t="s">
         <v>74</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-      <c r="L54" s="66"/>
-      <c r="N54" s="67" t="s">
+      <c r="L54" s="64"/>
+      <c r="N54" s="65" t="s">
         <v>63</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="66"/>
-    </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B55" s="69" t="s">
+      <c r="R54" s="64"/>
+      <c r="U54" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="22"/>
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B55" s="67" t="s">
         <v>115</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="66"/>
-      <c r="H55" s="67"/>
+      <c r="F55" s="64"/>
+      <c r="H55" s="65"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="66"/>
-      <c r="N55" s="67" t="s">
+      <c r="L55" s="64"/>
+      <c r="N55" s="65" t="s">
         <v>64</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="66"/>
-    </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="67"/>
+      <c r="R55" s="64"/>
+      <c r="U55" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="22"/>
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B56" s="65"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="66"/>
-      <c r="H56" s="68" t="s">
+      <c r="F56" s="64"/>
+      <c r="H56" s="66" t="s">
         <v>52</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="66"/>
-      <c r="N56" s="67"/>
+      <c r="L56" s="64"/>
+      <c r="N56" s="65"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="66"/>
-    </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B57" s="70" t="s">
+      <c r="R56" s="64"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+      <c r="Y56" s="22"/>
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B57" s="68" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="66"/>
-      <c r="H57" s="75" t="s">
+      <c r="F57" s="64"/>
+      <c r="H57" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="54"/>
-      <c r="L57" s="66"/>
-      <c r="N57" s="71" t="s">
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="64"/>
+      <c r="N57" s="69" t="s">
         <v>67</v>
       </c>
       <c r="O57" s="47"/>
       <c r="P57" s="47"/>
       <c r="Q57" s="48"/>
-      <c r="R57" s="66"/>
-    </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B58" s="72"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="74"/>
-      <c r="H58" s="69" t="s">
+      <c r="R57" s="64"/>
+      <c r="U57" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="V57" s="11"/>
+      <c r="W57" s="11"/>
+      <c r="X57" s="11"/>
+      <c r="Y57" s="22"/>
+    </row>
+    <row r="58" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B58" s="70"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
+      <c r="F58" s="72"/>
+      <c r="H58" s="67" t="s">
         <v>73</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="66"/>
-      <c r="N58" s="67"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="64"/>
+      <c r="N58" s="65"/>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
-      <c r="R58" s="66"/>
-    </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H59" s="76" t="s">
+      <c r="R58" s="64"/>
+      <c r="U58" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+      <c r="Y58" s="22"/>
+    </row>
+    <row r="59" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H59" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="59"/>
-      <c r="L59" s="66"/>
-      <c r="N59" s="70" t="s">
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="64"/>
+      <c r="N59" s="68" t="s">
         <v>117</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
-      <c r="R59" s="66"/>
-    </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H60" s="67"/>
+      <c r="R59" s="64"/>
+      <c r="U59" s="36"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2"/>
+      <c r="Y59" s="22"/>
+    </row>
+    <row r="60" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H60" s="65"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
-      <c r="L60" s="66"/>
-      <c r="N60" s="72"/>
-      <c r="O60" s="73"/>
-      <c r="P60" s="73"/>
-      <c r="Q60" s="73"/>
-      <c r="R60" s="74"/>
-    </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H61" s="63" t="s">
+      <c r="L60" s="64"/>
+      <c r="N60" s="70"/>
+      <c r="O60" s="71"/>
+      <c r="P60" s="71"/>
+      <c r="Q60" s="71"/>
+      <c r="R60" s="72"/>
+      <c r="U60" s="28"/>
+      <c r="V60" s="2"/>
+      <c r="W60" s="2"/>
+      <c r="X60" s="2"/>
+      <c r="Y60" s="22"/>
+    </row>
+    <row r="61" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H61" s="61" t="s">
         <v>17</v>
       </c>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
       <c r="K61" s="14"/>
-      <c r="L61" s="64"/>
-    </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H62" s="67"/>
+      <c r="L61" s="62"/>
+      <c r="U61" s="28"/>
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+      <c r="X61" s="2"/>
+      <c r="Y61" s="22"/>
+    </row>
+    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H62" s="65"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="66"/>
-    </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H63" s="68" t="s">
+      <c r="L62" s="64"/>
+      <c r="U62" s="28"/>
+      <c r="V62" s="2"/>
+      <c r="W62" s="2"/>
+      <c r="X62" s="2"/>
+      <c r="Y62" s="22"/>
+    </row>
+    <row r="63" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H63" s="66" t="s">
         <v>58</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-      <c r="L63" s="66"/>
-    </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="H64" s="77" t="s">
+      <c r="L63" s="64"/>
+      <c r="U63" s="28"/>
+      <c r="V63" s="2"/>
+      <c r="W63" s="2"/>
+      <c r="X63" s="2"/>
+      <c r="Y63" s="22"/>
+    </row>
+    <row r="64" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="H64" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="I64" s="53"/>
-      <c r="J64" s="53"/>
-      <c r="K64" s="54"/>
-      <c r="L64" s="66"/>
-    </row>
-    <row r="65" spans="8:18" x14ac:dyDescent="0.2">
-      <c r="H65" s="69" t="s">
+      <c r="I64" s="51"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="52"/>
+      <c r="L64" s="64"/>
+      <c r="U64" s="28"/>
+      <c r="V64" s="2"/>
+      <c r="W64" s="2"/>
+      <c r="X64" s="2"/>
+      <c r="Y64" s="22"/>
+    </row>
+    <row r="65" spans="8:25" x14ac:dyDescent="0.2">
+      <c r="H65" s="67" t="s">
         <v>76</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
-      <c r="K65" s="55"/>
-      <c r="L65" s="66"/>
-    </row>
-    <row r="66" spans="8:18" x14ac:dyDescent="0.2">
-      <c r="H66" s="76" t="s">
+      <c r="K65" s="53"/>
+      <c r="L65" s="64"/>
+      <c r="U65" s="29"/>
+      <c r="V65" s="30"/>
+      <c r="W65" s="30"/>
+      <c r="X65" s="30"/>
+      <c r="Y65" s="31"/>
+    </row>
+    <row r="66" spans="8:25" x14ac:dyDescent="0.2">
+      <c r="H66" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
-      <c r="K66" s="57"/>
-      <c r="L66" s="66"/>
-    </row>
-    <row r="67" spans="8:18" x14ac:dyDescent="0.2">
-      <c r="H67" s="67"/>
+      <c r="I66" s="54"/>
+      <c r="J66" s="54"/>
+      <c r="K66" s="55"/>
+      <c r="L66" s="64"/>
+    </row>
+    <row r="67" spans="8:25" x14ac:dyDescent="0.2">
+      <c r="H67" s="65"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-      <c r="L67" s="66"/>
-    </row>
-    <row r="68" spans="8:18" x14ac:dyDescent="0.2">
-      <c r="H68" s="70" t="s">
+      <c r="L67" s="64"/>
+    </row>
+    <row r="68" spans="8:25" x14ac:dyDescent="0.2">
+      <c r="H68" s="68" t="s">
         <v>117</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
-      <c r="L68" s="66"/>
-    </row>
-    <row r="69" spans="8:18" x14ac:dyDescent="0.2">
-      <c r="H69" s="72"/>
-      <c r="I69" s="73"/>
-      <c r="J69" s="73"/>
-      <c r="K69" s="73"/>
-      <c r="L69" s="74"/>
-    </row>
-    <row r="73" spans="8:18" x14ac:dyDescent="0.2">
+      <c r="L68" s="64"/>
+    </row>
+    <row r="69" spans="8:25" x14ac:dyDescent="0.2">
+      <c r="H69" s="70"/>
+      <c r="I69" s="71"/>
+      <c r="J69" s="71"/>
+      <c r="K69" s="71"/>
+      <c r="L69" s="72"/>
+    </row>
+    <row r="73" spans="8:25" x14ac:dyDescent="0.2">
       <c r="N73" s="11"/>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
     </row>
-    <row r="74" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="8:25" x14ac:dyDescent="0.2">
       <c r="N74" s="11"/>
       <c r="O74" s="11"/>
       <c r="P74" s="11"/>
       <c r="Q74" s="11"/>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="8:25" x14ac:dyDescent="0.2">
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="8:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="8:25" x14ac:dyDescent="0.2">
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>

</xml_diff>